<commit_message>
Correct L4 and L5 to 2.2uH. Update BOM
</commit_message>
<xml_diff>
--- a/hovImuBoard_BOM.xlsx
+++ b/hovImuBoard_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="151">
   <si>
     <t xml:space="preserve">    C5</t>
   </si>
@@ -179,12 +179,6 @@
     <t>AVR-JTAG-10</t>
   </si>
   <si>
-    <t>A33175-ND</t>
-  </si>
-  <si>
-    <t>5104338-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">    L1</t>
   </si>
   <si>
@@ -227,15 +221,6 @@
     <t>&gt;  L4, L5</t>
   </si>
   <si>
-    <t>22uH</t>
-  </si>
-  <si>
-    <t>587-3608-1-ND</t>
-  </si>
-  <si>
-    <t>NRS5040T220MMGKV</t>
-  </si>
-  <si>
     <t xml:space="preserve">    R1</t>
   </si>
   <si>
@@ -387,6 +372,111 @@
   </si>
   <si>
     <t>ECS Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    H1</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    J2</t>
+  </si>
+  <si>
+    <t>Ext. Power</t>
+  </si>
+  <si>
+    <t>SAM10711-ND</t>
+  </si>
+  <si>
+    <t>SHF-105-01-L-D-TH</t>
+  </si>
+  <si>
+    <t>Samtec Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    J5</t>
+  </si>
+  <si>
+    <t>ExtensionPort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    J6</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    JP17</t>
+  </si>
+  <si>
+    <t>0x69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    JP18</t>
+  </si>
+  <si>
+    <t>0x68</t>
+  </si>
+  <si>
+    <t>&gt;  JP19, JP20</t>
+  </si>
+  <si>
+    <t>Jumper_2_Bridged</t>
+  </si>
+  <si>
+    <t>2.2uH</t>
+  </si>
+  <si>
+    <t>587-2552-1-ND</t>
+  </si>
+  <si>
+    <t>NRS5012T2R2MMGF</t>
+  </si>
+  <si>
+    <t>&gt;  LOGO1, LOGO2</t>
+  </si>
+  <si>
+    <t>Logo_Open_Hardware_Small</t>
+  </si>
+  <si>
+    <t>541-200CCT-ND</t>
+  </si>
+  <si>
+    <t>CRCW0805200RFKEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    TP1</t>
+  </si>
+  <si>
+    <t>+3.3V_IMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    TP2</t>
+  </si>
+  <si>
+    <t>+12V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    TP3</t>
+  </si>
+  <si>
+    <t>+5V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    TP4</t>
+  </si>
+  <si>
+    <t>+3.3V</t>
+  </si>
+  <si>
+    <t>377-1757-ND</t>
+  </si>
+  <si>
+    <t>CU-1935-MB</t>
+  </si>
+  <si>
+    <t>Bud Industries</t>
   </si>
 </sst>
 </file>
@@ -704,18 +794,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -736,7 +825,7 @@
         <v>4</v>
       </c>
       <c r="F1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -756,7 +845,7 @@
         <v>4</v>
       </c>
       <c r="F2">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,7 +865,7 @@
         <v>4</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,7 +885,7 @@
         <v>17</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,7 +905,7 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -836,7 +925,7 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -856,7 +945,7 @@
         <v>30</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -876,7 +965,7 @@
         <v>35</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,407 +985,548 @@
         <v>35</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="F16">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18">
-        <v>155</v>
-      </c>
-      <c r="C18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" t="s">
-        <v>74</v>
+        <v>129</v>
+      </c>
+      <c r="B18" t="s">
+        <v>130</v>
       </c>
       <c r="F18">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20">
-        <v>150</v>
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="F20">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="F21">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="F23">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
-      </c>
-      <c r="B26" t="s">
-        <v>105</v>
+        <v>70</v>
+      </c>
+      <c r="B26">
+        <v>200</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="E26" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="F26">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="F27">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" t="s">
-        <v>113</v>
+        <v>75</v>
+      </c>
+      <c r="B28">
+        <v>150</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="F29">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" t="s">
+        <v>147</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" t="s">
+        <v>110</v>
+      </c>
+      <c r="E40" t="s">
+        <v>98</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>